<commit_message>
letzte anpassungen DV-Konzept, prozessdoku usw
</commit_message>
<xml_diff>
--- a/tasklogs/IAA-Tasklog-Gruppe11-NinaPick.xlsx
+++ b/tasklogs/IAA-Tasklog-Gruppe11-NinaPick.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NinaP\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NinaP\Documents\Uni\PraxisderSoftwareentwicklung\iaa_hausarbeit_nicht_stolarczyk_pick_gottschalk\tasklogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126D3330-6440-4947-991A-745E26924088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9089770-6473-4956-9A18-ECF29E4E61A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasklog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Tasklog</t>
   </si>
@@ -62,22 +62,13 @@
     <t>Erstellen ersten Service und Komponente für Tickets und Projekte im Frontend, Anzeige Testtickets aus Backend und erstellen anschaulicher Ticket/ Projekt-Liste im Frontend</t>
   </si>
   <si>
-    <t>Registrierung angepasst: Vor- und Nachnamen als Pflichtfelder im Registrierungsdialog ergänzt, Rolle Developer als Default Zuweisung</t>
-  </si>
-  <si>
     <t>Meeting:Aktueller Stand</t>
   </si>
   <si>
     <t xml:space="preserve">Meeting </t>
   </si>
   <si>
-    <t>Rework: Durchstich mit neuer Struktur im Frontend</t>
-  </si>
-  <si>
     <t>Tickets: initiale Create und Delete Funktion in Ticket-Liste Ansicht implementiert mit Dialog, sowie Routing bei Ausführungsfehler angepasst (keine default Weiterleitung zur Ticket-Liste); Update Funktion mit Inline-Editieren in Ticket-Detail Ansicht implementiert</t>
-  </si>
-  <si>
-    <t>Projekte: intiale Create und Delete Funktion in Projekt-Liste Ansicht implementiert mit Dialog, sowie Routing bei Ausführungsfehler angepasst (keine default Weiterleitung zur Ticket-Liste); Update Funktion mit Inline-Editieren in Projekt-Detail Ansicht implementiert</t>
   </si>
   <si>
     <t>Zusätze: eigene user-select Komponente für Suche/Auswahl existierender Developer User (Einsatz bei create Ticket), eigene project-select Komponente für Drop-Down Auswahl existierender Projekte (Einsatz bei create Ticket)</t>
@@ -113,13 +104,28 @@
     <t>kleinere Anpassungen: bei Page Sortierung der Listen Ansichten den Creator rausgenommen, reload bei Projektlöschung eingebaut, weitere Dokumentation im Code, READ ME Frontend-seitig ergänzt</t>
   </si>
   <si>
-    <t>Testfall Übersicht des Frontends erarbeitet</t>
-  </si>
-  <si>
     <t>Kommentare: Create Funktion für Kommentare für neue Parents-Kommentare und für Child-Kommentare</t>
   </si>
   <si>
     <t>Dialogflussmodell erstellt, KI-Doku, DV Konzept finalisiert</t>
+  </si>
+  <si>
+    <t>Einlesen in Frontendtechnologien: Angular, Tailwindcss und Daisyui</t>
+  </si>
+  <si>
+    <t>Erste Überlegungen Frontend Umsetzung, Struktur, Masken, Dialogflüsse</t>
+  </si>
+  <si>
+    <t>Testfall Übersicht des Frontends erarbeitet, kleinere bug fixes</t>
+  </si>
+  <si>
+    <t>Rework: Durchstich mit neuer Struktur im Frontend, Pairprogramming</t>
+  </si>
+  <si>
+    <t>Registrierung angepasst: Vor- und Nachnamen als Pflichtfelder im Registrierungsdialog ergänzt, Rolle Developer als Default Zuweisung, Pair Programming</t>
+  </si>
+  <si>
+    <t>Projekte: intiale Create und Delete Funktion in Projekt-Liste Ansicht implementiert mit Dialog, sowie Routing bei Ausführungsfehler angepasst (keine default Weiterleitung zur Ticket-Liste); Update Funktion mit Inline-Editieren in Projekt-Detail Ansicht implementiert, Pair Programming</t>
   </si>
 </sst>
 </file>
@@ -548,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z900"/>
+  <dimension ref="A1:Z902"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -662,13 +668,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
-        <v>45956</v>
+        <v>45952</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -696,13 +702,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
-        <v>45957</v>
+        <v>45954</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C5" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -728,15 +734,15 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>45959</v>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>45956</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>7</v>
+      <c r="B6" s="19" t="s">
+        <v>8</v>
       </c>
       <c r="C6" s="13">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -764,13 +770,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
-        <v>45960</v>
+        <v>45957</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C7" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -796,15 +802,15 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
-        <v>45965</v>
+    <row r="8" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>45959</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>4</v>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="13">
-        <v>0.75</v>
+        <v>4</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -830,15 +836,15 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>45969</v>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="18">
+        <v>45960</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>15</v>
+      <c r="B9" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -865,14 +871,14 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>45969</v>
+      <c r="A10" s="18">
+        <v>45965</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>11</v>
+      <c r="B10" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="C10" s="13">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -900,13 +906,13 @@
     </row>
     <row r="11" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C11" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -932,15 +938,15 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>45970</v>
+        <v>45969</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C12" s="13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -966,15 +972,15 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>45970</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>12</v>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
       </c>
-      <c r="C13" s="16">
-        <v>5</v>
+      <c r="C13" s="13">
+        <v>1</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1000,15 +1006,15 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>45970</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>14</v>
+      <c r="B14" s="6" t="s">
+        <v>29</v>
       </c>
-      <c r="C14" s="16">
-        <v>4</v>
+      <c r="C14" s="13">
+        <v>5</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1034,15 +1040,15 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
     </row>
-    <row r="15" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>45971</v>
+    <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>45970</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C15" s="16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1068,12 +1074,12 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>45971</v>
+    <row r="16" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>45970</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C16" s="16">
         <v>4</v>
@@ -1102,12 +1108,12 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
-        <v>45974</v>
+        <v>45971</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C17" s="16">
         <v>3</v>
@@ -1136,15 +1142,15 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
-        <v>45975</v>
+        <v>45971</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C18" s="16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1170,15 +1176,15 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
-        <v>45975</v>
+        <v>45974</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C19" s="16">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1204,15 +1210,15 @@
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
     </row>
-    <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>45975</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C20" s="16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -1243,10 +1249,10 @@
         <v>45975</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C21" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
@@ -1277,10 +1283,10 @@
         <v>45975</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C22" s="16">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1308,13 +1314,13 @@
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C23" s="16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1340,15 +1346,15 @@
       <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
     </row>
-    <row r="24" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
-        <v>45976</v>
+        <v>45975</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" s="16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1379,10 +1385,10 @@
         <v>45976</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C25" s="16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1408,15 +1414,15 @@
       <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
     </row>
-    <row r="26" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>45976</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C26" s="16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1442,14 +1448,15 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10" t="s">
-        <v>5</v>
+    <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
+        <v>45976</v>
       </c>
-      <c r="C27" s="11">
-        <f>SUM(C3:C26)</f>
-        <v>66.5</v>
+      <c r="B27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="16">
+        <v>3</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1475,10 +1482,16 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="14"/>
+    <row r="28" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12">
+        <v>45976</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="16">
+        <v>3</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1503,10 +1516,15 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="14"/>
+    <row r="29" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="11">
+        <f>SUM(C3:C28)</f>
+        <v>80</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -25919,6 +25937,62 @@
       <c r="Y900" s="3"/>
       <c r="Z900" s="3"/>
     </row>
+    <row r="901" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A901" s="3"/>
+      <c r="B901" s="2"/>
+      <c r="C901" s="14"/>
+      <c r="D901" s="3"/>
+      <c r="E901" s="3"/>
+      <c r="F901" s="3"/>
+      <c r="G901" s="3"/>
+      <c r="H901" s="3"/>
+      <c r="I901" s="3"/>
+      <c r="J901" s="3"/>
+      <c r="K901" s="3"/>
+      <c r="L901" s="3"/>
+      <c r="M901" s="3"/>
+      <c r="N901" s="3"/>
+      <c r="O901" s="3"/>
+      <c r="P901" s="3"/>
+      <c r="Q901" s="3"/>
+      <c r="R901" s="3"/>
+      <c r="S901" s="3"/>
+      <c r="T901" s="3"/>
+      <c r="U901" s="3"/>
+      <c r="V901" s="3"/>
+      <c r="W901" s="3"/>
+      <c r="X901" s="3"/>
+      <c r="Y901" s="3"/>
+      <c r="Z901" s="3"/>
+    </row>
+    <row r="902" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A902" s="3"/>
+      <c r="B902" s="2"/>
+      <c r="C902" s="14"/>
+      <c r="D902" s="3"/>
+      <c r="E902" s="3"/>
+      <c r="F902" s="3"/>
+      <c r="G902" s="3"/>
+      <c r="H902" s="3"/>
+      <c r="I902" s="3"/>
+      <c r="J902" s="3"/>
+      <c r="K902" s="3"/>
+      <c r="L902" s="3"/>
+      <c r="M902" s="3"/>
+      <c r="N902" s="3"/>
+      <c r="O902" s="3"/>
+      <c r="P902" s="3"/>
+      <c r="Q902" s="3"/>
+      <c r="R902" s="3"/>
+      <c r="S902" s="3"/>
+      <c r="T902" s="3"/>
+      <c r="U902" s="3"/>
+      <c r="V902" s="3"/>
+      <c r="W902" s="3"/>
+      <c r="X902" s="3"/>
+      <c r="Y902" s="3"/>
+      <c r="Z902" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>